<commit_message>
fix(CAN): correct value of CAN protocal sent to motor driver
</commit_message>
<xml_diff>
--- a/doc/ROV STM32下位机/ROV中CAN协议.xlsx
+++ b/doc/ROV STM32下位机/ROV中CAN协议.xlsx
@@ -123,7 +123,7 @@
     <t>操作模式</t>
   </si>
   <si>
-    <t>0/1</t>
+    <t>85/170</t>
   </si>
   <si>
     <t>UI测试/手柄遥控</t>
@@ -346,8 +346,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -366,23 +366,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -403,33 +397,24 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -443,22 +428,37 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -472,7 +472,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -487,23 +487,23 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -532,37 +532,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,139 +646,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,8 +775,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -786,6 +786,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -808,23 +823,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -874,148 +874,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="11" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="11" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="11" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="10" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1413,8 +1413,8 @@
   <sheetPr/>
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1" defaultRowHeight="18.4"/>

</xml_diff>